<commit_message>
sigma_s and sigma_t fixed
</commit_message>
<xml_diff>
--- a/data/landings.xlsx
+++ b/data/landings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dangranger/Documents/Both/Aviation/References/Courses/NTPS/NTPS 2024/Modules/Capstone/python/landing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B396E9-9FAA-7D4B-A358-428492014D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9939170A-4779-0742-881B-B1957EBE7DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18000" yWindow="660" windowWidth="17680" windowHeight="21580" activeTab="1" xr2:uid="{90425064-DA34-9B42-9B5B-0D6B8F053C02}"/>
   </bookViews>
@@ -542,7 +542,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -648,7 +648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4737AC-B4FA-A74F-84DF-3102D64B56E6}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -745,7 +745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E45E612-CA4A-B542-BB6E-DC23C33E78E0}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>

</xml_diff>